<commit_message>
Addition: adding test codes for instagram login amd registration using page object model
</commit_message>
<xml_diff>
--- a/src/main/Resources/Book1.xlsx
+++ b/src/main/Resources/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atulk\IdeaProjects\POM-Instagram\src\main\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1997AE32-4710-4E76-97A4-1AB1DDA8A16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCDCEB2-577D-43B2-AEF9-B653B19CF7AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{FE86F0B0-95F0-4350-9776-85F1BFEBEC3D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FE86F0B0-95F0-4350-9776-85F1BFEBEC3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Surabhisanjan05</t>
+    <t>Theend@1</t>
   </si>
   <si>
-    <t>Surabhi@1</t>
+    <t>TestingBLZ123</t>
   </si>
 </sst>
 </file>
@@ -416,10 +416,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>